<commit_message>
Have a Test case
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alcp2\IntelliJIDEAProjects\BubbleDex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13FF9D3-FE2A-4A00-96AA-F71C9C4FBE3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B630DF0-B9AC-4E50-87CC-ABF51FBCF4D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2330" yWindow="1410" windowWidth="14400" windowHeight="7820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Jonny</t>
   </si>
@@ -43,6 +43,60 @@
   </si>
   <si>
     <t>UGA</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Regiment 8</t>
+  </si>
+  <si>
+    <t>7/2016,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regiment </t>
+  </si>
+  <si>
+    <t>1/2015,6/2016</t>
+  </si>
+  <si>
+    <t>8/2011,5/2015</t>
+  </si>
+  <si>
+    <t>9/2005,8/2014</t>
+  </si>
+  <si>
+    <t>8/2000,5/2004</t>
+  </si>
+  <si>
+    <t>5/2015,9/2017</t>
+  </si>
+  <si>
+    <t>Parker</t>
+  </si>
+  <si>
+    <t>Regiment 4</t>
+  </si>
+  <si>
+    <t>Atlanta Symposium</t>
+  </si>
+  <si>
+    <t>3/2015,8/2018</t>
+  </si>
+  <si>
+    <t>2/2015,5/2016</t>
+  </si>
+  <si>
+    <t>Annie</t>
+  </si>
+  <si>
+    <t>5/2019,5/2019</t>
+  </si>
+  <si>
+    <t>6/2004,8/2007</t>
+  </si>
+  <si>
+    <t>5/2015,</t>
   </si>
 </sst>
 </file>
@@ -78,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,34 +415,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="11.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
         <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>